<commit_message>
EPICP-5 adjusted documents for harmonisation
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_EPICP_P2.xlsx
+++ b/rmonize/data_dictionary/DD_EPICP_P2.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -746,12 +746,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ff10</t>
+          <t>kind1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Total number of stillbirths</t>
+          <t>How old were you when you gave birth to your first child?</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -766,12 +766,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>kind1</t>
+          <t>prevcanc</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>How old were you when you gave birth to your first child?</t>
+          <t>prevalent cancer</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -786,12 +786,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>prevcanc</t>
+          <t>lipidlower</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>prevalent cancer</t>
+          <t>Lipid-lowering drugs</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -806,12 +806,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>lipidlower</t>
+          <t>nsar_excl_ASS</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Lipid-lowering drugs</t>
+          <t>non-steroidal anti-inflammatory drug (excl.ASS)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -826,12 +826,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>nsar_excl_ASS</t>
+          <t>casemi_fup5</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>non-steroidal anti-inflammatory drug (excl.ASS)</t>
+          <t>case status of myocardial infarction at FUP5</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -846,12 +846,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>casemi_fup5</t>
+          <t>casestroke_fup5</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>case status of myocardial infarction at FUP5</t>
+          <t>case status of stroke at FUP5</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -866,17 +866,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>casestroke_fup5</t>
+          <t>dd_incmi</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>case status of stroke at FUP5</t>
+          <t>date of diagnosis of myocardial infarction</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>date</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>dd_incmi</t>
+          <t>dd_incstroke</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>date of diagnosis of myocardial infarction</t>
+          <t>date of diagnosis of stroke</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -906,17 +906,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>dd_incstroke</t>
+          <t>caseI63_fup5</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>date of diagnosis of stroke</t>
+          <t>ischaemic insult (ICD-10 I63)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>integer</t>
         </is>
       </c>
     </row>
@@ -926,12 +926,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>caseI63_fup5</t>
+          <t>caseI61_fup5</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ischaemic insult (ICD-10 I63)</t>
+          <t>intracerebral hemorrhage (ICD-10 I61)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -946,12 +946,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>caseI61_fup5</t>
+          <t>casehyp_fup5</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>intracerebral hemorrhage (ICD-10 I61)</t>
+          <t>case status of essential hypertension at FUP5</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -966,17 +966,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>casehyp_fup5</t>
+          <t>dd_inchyp</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>case status of essential hypertension at FUP5</t>
+          <t>date of diagnosis of essential hypertension</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>date</t>
         </is>
       </c>
     </row>
@@ -986,17 +986,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>dd_inchyp</t>
+          <t>casehf_fup5</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>date of diagnosis of essential hypertension</t>
+          <t>case status of heart failure at FUP5</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>integer</t>
         </is>
       </c>
     </row>
@@ -1006,17 +1006,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>casehf_fup5</t>
+          <t>dd_inchf</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>case status of heart failure at FUP5</t>
+          <t>date of diagnosis of heart failure</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>date</t>
         </is>
       </c>
     </row>
@@ -1026,17 +1026,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>dd_inchf</t>
+          <t>casediab_fup5</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>date of diagnosis of heart failure</t>
+          <t>case status of diabetes at FUP5</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>integer</t>
         </is>
       </c>
     </row>
@@ -1046,17 +1046,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>casediab_fup5</t>
+          <t>dd_incdiab</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>case status of diabetes at FUP5</t>
+          <t>date of diagnosis of diabetes</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>date</t>
         </is>
       </c>
     </row>
@@ -1066,17 +1066,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>dd_incdiab</t>
+          <t>inccanc_fup5</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>date of diagnosis of diabetes</t>
+          <t>incident first occuring cancer at FUP5</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>integer</t>
         </is>
       </c>
     </row>
@@ -1086,17 +1086,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>inccanc_fup5</t>
+          <t>dd_inccanc</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>incident first occuring cancer at FUP5</t>
+          <t>date of diagnosis of first occuring cancer</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>date</t>
         </is>
       </c>
     </row>
@@ -1106,17 +1106,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>dd_inccanc</t>
+          <t>vitstat5</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>date of diagnosis of first occuring cancer</t>
+          <t>vital status at FUP5</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>integer</t>
         </is>
       </c>
     </row>
@@ -1126,17 +1126,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>vitstat5</t>
+          <t>age_death</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>vital status at FUP5</t>
+          <t>age of death</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>decimal</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>age_death</t>
+          <t>age_fup5</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>age of death</t>
+          <t>age at FUP5</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1166,12 +1166,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>age_fup5</t>
+          <t>bmi0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>age at FUP5</t>
+          <t>BMI at baseline</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1186,12 +1186,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>bmi0</t>
+          <t>bmi_f4</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BMI at baseline</t>
+          <t>BMI at FUP4</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>bmi_f4</t>
+          <t>waist0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BMI at FUP4</t>
+          <t>waist circumference at baseline [cm]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>waist0</t>
+          <t>hip0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>waist circumference at baseline [cm]</t>
+          <t>hip circumference at baseline [cm]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1246,12 +1246,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>hip0</t>
+          <t>waist_f4</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>hip circumference at baseline [cm]</t>
+          <t>waist circumference at FUP4 [cm]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>waist_f4</t>
+          <t>hip_f4</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>waist circumference at FUP4 [cm]</t>
+          <t>hip circumference at FUP4 [cm]</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1286,12 +1286,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>hip_f4</t>
+          <t>age_anth_f4</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>hip circumference at FUP4 [cm]</t>
+          <t>age of anthropometric measurement at FUP4</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1306,12 +1306,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>age_anth_f4</t>
+          <t>GJ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>age of anthropometric measurement at FUP4</t>
+          <t>Total energy intake at baseline [kJ/d]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1326,12 +1326,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>GJ</t>
+          <t>corr_trigly</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Total energy intake at baseline [kJ/d]</t>
+          <t>corrected triglycerides [mg/dL]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1346,12 +1346,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>corr_trigly</t>
+          <t>corr_chol</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>corrected triglycerides [mg/dL]</t>
+          <t>corrected cholesterol [mg/dL]</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1366,12 +1366,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>corr_chol</t>
+          <t>corr_hdl</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>corrected cholesterol [mg/dL]</t>
+          <t>corrected HDL cholesterol [mg/dL]</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>corr_hdl</t>
+          <t>ZK</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>corrected HDL cholesterol [mg/dL]</t>
+          <t>carbohydrate intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1406,12 +1406,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ZK</t>
+          <t>ZE</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>carbohydrate intake at baseline [g/d]</t>
+          <t>protein intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ZE</t>
+          <t>ZF</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>protein intake at baseline [g/d]</t>
+          <t>fat intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ZF</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>fat intake at baseline [g/d]</t>
+          <t>alcohol intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1466,12 +1466,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>ZB</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>alcohol intake at baseline [g/d]</t>
+          <t>fiber intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ZB</t>
+          <t>FS</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>fiber intake at baseline [g/d]</t>
+          <t>saturated fatty acid intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1506,12 +1506,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>FU</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>saturated fatty acid intake at baseline [g/d]</t>
+          <t>monounsaturated fatty acid intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1526,12 +1526,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>FU</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>monounsaturated fatty acid intake at baseline [g/d]</t>
+          <t>polyunsaturated fatty acid intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>KD</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>polyunsaturated fatty acid intake at baseline [g/d]</t>
+          <t>disaccharide intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>KD</t>
+          <t>KM</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>disaccharide intake at baseline [g/d]</t>
+          <t>monosaccharide intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>KM</t>
+          <t>KMT</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>monosaccharide intake at baseline [g/d]</t>
+          <t>glucose intakeat baseline [g/d]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1606,12 +1606,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>KMT</t>
+          <t>KMF</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>glucose intakeat baseline [g/d]</t>
+          <t>fructose intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>KMF</t>
+          <t>MNA</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>fructose intake at baseline [g/d]</t>
+          <t>sodium intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1646,12 +1646,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>MNA</t>
+          <t>MK</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>sodium intake at baseline [g/d]</t>
+          <t>potassium intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MK</t>
+          <t>VEGETABLES_02</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>potassium intake at baseline [g/d]</t>
+          <t>Vegetable intake [g/d]</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1686,12 +1686,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>VEGETABLES_02</t>
+          <t>LEGUMES_TOT_03</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Vegetable intake [g/d]</t>
+          <t>Total legumes intake [g/d]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1706,12 +1706,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>LEGUMES_TOT_03</t>
+          <t>FRUITS_TOT_04</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Total legumes intake [g/d]</t>
+          <t>Total fruit intake [g/d]</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1726,12 +1726,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>FRUITS_TOT_04</t>
+          <t>RED_MEAT_0701</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Total fruit intake [g/d]</t>
+          <t>Intake of red meat (mammals meat) [g/d]</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1746,12 +1746,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>RED_MEAT_0701</t>
+          <t>PROCMEAT_0704</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Intake of red meat (mammals meat) [g/d]</t>
+          <t>Intake of processed or preserved meat [g/d]</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>PROCMEAT_0704</t>
+          <t>SUGAR_CONFECT_11</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Intake of processed or preserved meat [g/d]</t>
+          <t>Intake of sugar and similar, confectionery and water-based sweet desserts [g/d]</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1786,12 +1786,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>SUGAR_CONFECT_11</t>
+          <t>CAKES_12</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Intake of sugar and similar, confectionery and water-based sweet desserts [g/d]</t>
+          <t>Intake of cakes and fine bakery products [g/d]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1806,12 +1806,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CAKES_12</t>
+          <t>FRUITVEG_JUICE_1301</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Intake of cakes and fine bakery products [g/d]</t>
+          <t>Intake of fruit and vegetable juices [g/d]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1826,12 +1826,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>FRUITVEG_JUICE_1301</t>
+          <t>SOFTDRINKS_1302</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Intake of fruit and vegetable juices [g/d]</t>
+          <t>Intake of soft drinks [g/d]</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1846,12 +1846,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>SOFTDRINKS_1302</t>
+          <t>COFFEE_130301</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Intake of soft drinks [g/d]</t>
+          <t>Coffee intake [g/d]</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1866,12 +1866,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>COFFEE_130301</t>
+          <t>TEA_130302</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Coffee intake [g/d]</t>
+          <t>Tea intake [g/d]</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1886,35 +1886,15 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>TEA_130302</t>
+          <t>ART_SWEETENER_170201</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Tea intake [g/d]</t>
+          <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
-        <is>
-          <t>decimal</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>ART_SWEETENER_170201</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
         <is>
           <t>decimal</t>
         </is>

</xml_diff>

<commit_message>
EPICP-5 finalising the rmonize files
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_EPICP_P2.xlsx
+++ b/rmonize/data_dictionary/DD_EPICP_P2.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>inccanc_fup5</t>
+          <t>inccanc</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1166,17 +1166,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>inccanc</t>
+          <t>dcens_canc</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>incident first occuring cancer</t>
+          <t>censored date for cancer at FUP5</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>date</t>
         </is>
       </c>
     </row>
@@ -1186,17 +1186,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>dcens_canc</t>
+          <t>bmi0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>censored age for cancer at FUP5</t>
+          <t>BMI at baseline</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>decimal</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>bmi0</t>
+          <t>bmi_f4</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BMI at baseline</t>
+          <t>BMI at FUP4</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>bmi_f4</t>
+          <t>waist0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>BMI at FUP4</t>
+          <t>waist circumference at baseline [cm]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1246,12 +1246,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>waist0</t>
+          <t>hip0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>waist circumference at baseline [cm]</t>
+          <t>hip circumference at baseline [cm]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>hip0</t>
+          <t>waist_f4</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>hip circumference at baseline [cm]</t>
+          <t>waist circumference at FUP4 [cm]</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1286,12 +1286,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>waist_f4</t>
+          <t>hip_f4</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>waist circumference at FUP4 [cm]</t>
+          <t>hip circumference at FUP4 [cm]</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1306,12 +1306,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>hip_f4</t>
+          <t>age_anth_f4</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>hip circumference at FUP4 [cm]</t>
+          <t>age of anthropometric measurement at FUP4</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1326,12 +1326,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>age_anth_f4</t>
+          <t>GJ</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>age of anthropometric measurement at FUP4</t>
+          <t>Total energy intake at baseline [kJ/d]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1346,12 +1346,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>GJ</t>
+          <t>corr_trigly</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Total energy intake at baseline [kJ/d]</t>
+          <t>corrected triglycerides [mg/dL]</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1366,12 +1366,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>corr_trigly</t>
+          <t>corr_chol</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>corrected triglycerides [mg/dL]</t>
+          <t>corrected cholesterol [mg/dL]</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>corr_chol</t>
+          <t>corr_hdl</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>corrected cholesterol [mg/dL]</t>
+          <t>corrected HDL cholesterol [mg/dL]</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1406,12 +1406,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>corr_hdl</t>
+          <t>ZK</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>corrected HDL cholesterol [mg/dL]</t>
+          <t>carbohydrate intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ZK</t>
+          <t>ZE</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>carbohydrate intake at baseline [g/d]</t>
+          <t>protein intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ZE</t>
+          <t>ZF</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>protein intake at baseline [g/d]</t>
+          <t>fat intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1466,12 +1466,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ZF</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>fat intake at baseline [g/d]</t>
+          <t>alcohol intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>ZB</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>alcohol intake at baseline [g/d]</t>
+          <t>fiber intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1506,12 +1506,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ZB</t>
+          <t>FS</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>fiber intake at baseline [g/d]</t>
+          <t>saturated fatty acid intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1526,12 +1526,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>FU</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>saturated fatty acid intake at baseline [g/d]</t>
+          <t>monounsaturated fatty acid intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>FU</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>monounsaturated fatty acid intake at baseline [g/d]</t>
+          <t>polyunsaturated fatty acid intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>KD</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>polyunsaturated fatty acid intake at baseline [g/d]</t>
+          <t>disaccharide intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>KD</t>
+          <t>KM</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>disaccharide intake at baseline [g/d]</t>
+          <t>monosaccharide intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1606,12 +1606,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>KM</t>
+          <t>KMT</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>monosaccharide intake at baseline [g/d]</t>
+          <t>glucose intakeat baseline [g/d]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>KMT</t>
+          <t>KMF</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>glucose intakeat baseline [g/d]</t>
+          <t>fructose intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1646,12 +1646,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>KMF</t>
+          <t>MNA</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>fructose intake at baseline [g/d]</t>
+          <t>sodium intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MNA</t>
+          <t>MK</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>sodium intake at baseline [g/d]</t>
+          <t>potassium intake at baseline [g/d]</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1686,12 +1686,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>MK</t>
+          <t>VEGETABLES_02</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>potassium intake at baseline [g/d]</t>
+          <t>Vegetable intake [g/d]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1706,12 +1706,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>VEGETABLES_02</t>
+          <t>LEGUMES_TOT_03</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Vegetable intake [g/d]</t>
+          <t>Total legumes intake [g/d]</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1726,12 +1726,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>LEGUMES_TOT_03</t>
+          <t>FRUITS_TOT_04</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Total legumes intake [g/d]</t>
+          <t>Total fruit intake [g/d]</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1746,12 +1746,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>FRUITS_TOT_04</t>
+          <t>RED_MEAT_0701</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Total fruit intake [g/d]</t>
+          <t>Intake of red meat (mammals meat) [g/d]</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>RED_MEAT_0701</t>
+          <t>PROCMEAT_0704</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Intake of red meat (mammals meat) [g/d]</t>
+          <t>Intake of processed or preserved meat [g/d]</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1786,12 +1786,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>PROCMEAT_0704</t>
+          <t>SUGAR_CONFECT_11</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Intake of processed or preserved meat [g/d]</t>
+          <t>Intake of sugar and similar, confectionery and water-based sweet desserts [g/d]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1806,12 +1806,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SUGAR_CONFECT_11</t>
+          <t>CAKES_12</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Intake of sugar and similar, confectionery and water-based sweet desserts [g/d]</t>
+          <t>Intake of cakes and fine bakery products [g/d]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1826,12 +1826,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>CAKES_12</t>
+          <t>FRUITVEG_JUICE_1301</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Intake of cakes and fine bakery products [g/d]</t>
+          <t>Intake of fruit and vegetable juices [g/d]</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1846,12 +1846,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>FRUITVEG_JUICE_1301</t>
+          <t>SOFTDRINKS_1302</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Intake of fruit and vegetable juices [g/d]</t>
+          <t>Intake of soft drinks [g/d]</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1866,12 +1866,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SOFTDRINKS_1302</t>
+          <t>COFFEE_130301</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Intake of soft drinks [g/d]</t>
+          <t>Coffee intake [g/d]</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1886,12 +1886,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>COFFEE_130301</t>
+          <t>TEA_130302</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Coffee intake [g/d]</t>
+          <t>Tea intake [g/d]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1906,35 +1906,15 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>TEA_130302</t>
+          <t>ART_SWEETENER_170201</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Tea intake [g/d]</t>
+          <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
-        <is>
-          <t>decimal</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>ART_SWEETENER_170201</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
         <is>
           <t>decimal</t>
         </is>
@@ -1947,7 +1927,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2948,118 +2928,73 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>inccanc_fup5</t>
+          <t>vitstat5</t>
         </is>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>alive</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>inccanc_fup5</t>
+          <t>vitstat5</t>
         </is>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>dead</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>inccanc_fup5</t>
+          <t>vitstat5</t>
         </is>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>incident (not verif.)</t>
+          <t>dropped out</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>vitstat5</t>
+          <t>inccanc</t>
         </is>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>alive</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>vitstat5</t>
+          <t>inccanc</t>
         </is>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C71" t="inlineStr">
-        <is>
-          <t>dead</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>vitstat5</t>
-        </is>
-      </c>
-      <c r="B72">
-        <v>6</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>dropped out</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>inccanc</t>
-        </is>
-      </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>inccanc</t>
-        </is>
-      </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>